<commit_message>
update TC Delete user
</commit_message>
<xml_diff>
--- a/Testing/Test Report/TestCases.xlsx
+++ b/Testing/Test Report/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" activeTab="5"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="370">
   <si>
     <t>ID</t>
   </si>
@@ -655,14 +655,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1-user should have a browser to navigate to signup page.</t>
+      <t>1-admin should have a browser to navigate to signup page.</t>
     </r>
     <r>
       <rPr>
@@ -672,142 +665,19 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
+2-admin should have xampp and it's control panel
+3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+5- Admin is logged in and navigated to the delete user page</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2-User should have xampp and it's control panel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">3- user should have the database on the phpmyadmin (reach it through xampp control panel) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>4- open the apache server and sql server</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>5- Admin is logged in and navigated to the delete user page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Username:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" HasnaaAmed "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>E-mail :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" Hasnaa@yahoo.com "</t>
-    </r>
+  </si>
+  <si>
+    <t>1.fill fields in delete user page
+ Username:
+" HasnaaAmed "
+E-mail :
+" Hasnaa@yahoo.com "
+2.click on delete button</t>
   </si>
   <si>
     <r>
@@ -857,71 +727,29 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Username:</t>
+      <t>1-admin should have a browser to navigate to signup page.</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
+2-admin should have xampp and it's control panel
+3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+6- Admin is logged in and navigated to the delete user page</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" AdminAmed "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>E-mail :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" Ahmed@yahoo.com "</t>
-    </r>
+  </si>
+  <si>
+    <t>1.fill fields in delete user page
+Username:
+" AdminAmed "
+E-mail :
+" Ahmed@yahoo.com "
+2.click on delete button</t>
   </si>
   <si>
     <r>
@@ -998,71 +826,29 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Username:</t>
+      <t>1-admin should have a browser to navigate to signup page.</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
+2-admin should have xampp and it's control panel
+3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+7- Admin is logged in and navigated to the delete user page</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" HasnaaAmed# "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>E-mail :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" Hasnaa@yahoo.com "</t>
-    </r>
+  </si>
+  <si>
+    <t>1.fill fields in delete user page
+Username:
+" HasnaaAmed# "
+E-mail :
+" Hasnaa@yahoo.com "
+2.click on delete button</t>
   </si>
   <si>
     <r>
@@ -1148,71 +934,29 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Username:</t>
+      <t>1-admin should have a browser to navigate to signup page.</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
+2-admin should have xampp and it's control panel
+3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+8- Admin is logged in and navigated to the delete user page</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" HasnaaAmed22 "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>E-mail :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" Hasnaa@yahoo.com "</t>
-    </r>
+  </si>
+  <si>
+    <t>1.fill fields in delete user page
+Username:
+" HasnaaAmed22 "
+E-mail :
+" Hasnaa@yahoo.com "
+2.click on delete button</t>
   </si>
   <si>
     <t>TC_LearningHub_deleteuser_005</t>
@@ -1250,71 +994,29 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Username: </t>
+      <t>1-admin should have a browser to navigate to signup page.</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
+2-admin should have xampp and it's control panel
+3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+9- Admin is logged in and navigated to the delete user page</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">" HasnaaAmed " </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">E-mail : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>" Ahmed@yahoo.com "</t>
-    </r>
+  </si>
+  <si>
+    <t>1.fill fields in delete user page
+Username: 
+" HasnaaAmed " 
+E-mail : 
+" Ahmed@yahoo.com "
+2.click on delete button</t>
   </si>
   <si>
     <r>
@@ -1373,6 +1075,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>1-user should have a browser to navigate to signup page.</t>
     </r>
     <r>
@@ -1479,6 +1188,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>1-user should have a browser to navigate to signup page.</t>
     </r>
     <r>
@@ -1584,6 +1300,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>1-user should have a browser to navigate to signup page.</t>
     </r>
     <r>
@@ -2362,12 +2085,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2416,12 +2139,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
@@ -2455,16 +2172,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2472,7 +2182,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2493,16 +2210,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2524,6 +2241,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -2539,16 +2263,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2569,16 +2286,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2594,6 +2303,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2664,13 +2381,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2682,7 +2477,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2694,127 +2519,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2826,7 +2531,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2844,7 +2549,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3129,6 +2846,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3154,32 +2895,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -3197,32 +2912,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3232,131 +2949,131 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3399,97 +3116,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3501,7 +3218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3519,10 +3236,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3531,10 +3248,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3543,13 +3260,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="32" applyFont="1" applyAlignment="1">
@@ -4737,456 +4454,456 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>295</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A13" s="4" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A16" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>337</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A17" s="4" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A18" s="4" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A19" s="4" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A20" s="4" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>350</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A22" s="4" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A23" s="4" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A24" s="4" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>359</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A25" s="4" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -6865,7 +6582,7 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -6929,70 +6646,70 @@
         <v>161</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
     </row>
     <row r="4" ht="228" customHeight="1" spans="1:7">
       <c r="A4" s="37" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
     </row>
     <row r="5" ht="165.75" spans="1:7">
       <c r="A5" s="37" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B5" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="43" t="s">
         <v>169</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>167</v>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
     </row>
     <row r="6" ht="235.95" customHeight="1" spans="1:7">
       <c r="A6" s="37" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
@@ -7008,7 +6725,7 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -7048,76 +6765,76 @@
     </row>
     <row r="2" ht="199" customHeight="1" spans="1:7">
       <c r="A2" s="20" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" ht="195" customHeight="1" spans="1:7">
       <c r="A3" s="20" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
     <row r="4" ht="249" customHeight="1" spans="1:7">
       <c r="A4" s="20" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
     </row>
     <row r="5" ht="180.75" spans="1:7">
       <c r="A5" s="20" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>187</v>
-      </c>
       <c r="D5" s="26" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
@@ -7188,22 +6905,22 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A2" s="11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="11"/>
@@ -7212,22 +6929,22 @@
     </row>
     <row r="3" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A3" s="11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="13" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="11"/>
@@ -7236,22 +6953,22 @@
     </row>
     <row r="4" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="13" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="13" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="11"/>
@@ -7260,22 +6977,22 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="13" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="13" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="11"/>
@@ -7284,22 +7001,22 @@
     </row>
     <row r="6" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="11"/>
@@ -7308,22 +7025,22 @@
     </row>
     <row r="7" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="13" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="11"/>
@@ -7416,22 +7133,22 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A2" s="11" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="11"/>
@@ -7440,22 +7157,22 @@
     </row>
     <row r="3" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A3" s="11" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="13" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="11"/>
@@ -7464,22 +7181,22 @@
     </row>
     <row r="4" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="13" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="13" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="11"/>
@@ -7488,22 +7205,22 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>235</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="13" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="13" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="11"/>
@@ -7512,22 +7229,22 @@
     </row>
     <row r="6" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="11"/>
@@ -7612,260 +7329,260 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="96" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="91.2" customHeight="1" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>249</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="87" customHeight="1" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="102" customHeight="1" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="100.2" customHeight="1" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="99.6" customHeight="1" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="95.4" customHeight="1" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="94.2" customHeight="1" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="95.4" customHeight="1" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>278</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="94.2" customHeight="1" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="94.8" customHeight="1" spans="1:7">
       <c r="A13" s="4" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="102.6" customHeight="1" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="94.8" customHeight="1" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>274</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>

</xml_diff>

<commit_message>
update delete user TC after review
</commit_message>
<xml_diff>
--- a/Testing/Test Report/TestCases.xlsx
+++ b/Testing/Test Report/TestCases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="371">
   <si>
     <t>ID</t>
   </si>
@@ -651,7 +651,7 @@
     <t>TC_LearningHub_deleteuser_001</t>
   </si>
   <si>
-    <t>Valid Input - Delete Normal User</t>
+    <t>Valid Input - Delete User</t>
   </si>
   <si>
     <r>
@@ -668,56 +668,19 @@
 2-admin should have xampp and it's control panel
 3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
 4- open the apache server and sql server
-5- Admin is logged in and navigated to the delete user page</t>
+5- Admin is logged in and from dropdown menu in navbar choose "profile" then click on delete user.</t>
     </r>
   </si>
   <si>
     <t>1.fill fields in delete user page
- Username:
-" HasnaaAmed "
-E-mail :
-" Hasnaa@yahoo.com "
+Username: 
+johndoe
+Email: john@example.com
 2.click on delete button</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">user "normal" is deleted successfully </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">user is deleted from database and sucess  message appear "User deleted successfully..."
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">from the database. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>TC_LearningHub_deleteuser_002</t>
@@ -740,7 +703,7 @@
 2-admin should have xampp and it's control panel
 3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
 4- open the apache server and sql server
-6- Admin is logged in and navigated to the delete user page</t>
+6- Admin is logged in and from dropdown menu in navbar choose "profile" then click on delete user.</t>
     </r>
   </si>
   <si>
@@ -752,77 +715,15 @@
 2.click on delete button</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>user "Admin " is deleted successfully</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">sucess  message appear "User deleted successfully..."
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">from the database. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>TC_LearningHub_deleteuser_003</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Invalid Input - Username </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>contains special characters</t>
-    </r>
+    <t>Invalid Input - Username 
+doesn't exist in database</t>
   </si>
   <si>
     <r>
@@ -839,7 +740,7 @@
 2-admin should have xampp and it's control panel
 3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
 4- open the apache server and sql server
-7- Admin is logged in and navigated to the delete user page</t>
+7- Admin is logged in and from dropdown menu in navbar choose "profile" then click on delete user.</t>
     </r>
   </si>
   <si>
@@ -904,32 +805,17 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Invalid Input - Username</t>
+      <t>Invalid Input- email not attached to</t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>contains numbers</t>
+the entered username</t>
     </r>
   </si>
   <si>
@@ -947,73 +833,13 @@
 2-admin should have xampp and it's control panel
 3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
 4- open the apache server and sql server
-8- Admin is logged in and navigated to the delete user page</t>
-    </r>
-  </si>
-  <si>
-    <t>1.fill fields in delete user page
-Username:
-" HasnaaAmed22 "
-E-mail :
-" Hasnaa@yahoo.com "
-2.click on delete button</t>
-  </si>
-  <si>
-    <t>TC_LearningHub_deleteuser_005</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Invalid Input- not attached to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>the entered username</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1-admin should have a browser to navigate to signup page.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-2-admin should have xampp and it's control panel
-3- admin should have the database on the phpmyadmin (reach it through xampp control panel) 
-4- open the apache server and sql server
-9- Admin is logged in and navigated to the delete user page</t>
+9- Admin is logged in and from dropdown menu in navbar choose "profile" then click on delete user.</t>
     </r>
   </si>
   <si>
     <t>1.fill fields in delete user page
 Username: 
-" HasnaaAmed " 
+" johndoe" 
 E-mail : 
 " Ahmed@yahoo.com "
 2.click on delete button</t>
@@ -1066,6 +892,38 @@
       </rPr>
       <t>and the user will not be deleted.</t>
     </r>
+  </si>
+  <si>
+    <t>TC_LearningHub_deleteuser_005</t>
+  </si>
+  <si>
+    <t>Invalid User role</t>
+  </si>
+  <si>
+    <r>
+      <t>1-user should have a browser to navigate to signup page.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+2-user should have xampp and it's control panel
+3- user should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+5-user is logged in and from dropdown menu in navbar choose "profile".</t>
+    </r>
+  </si>
+  <si>
+    <t>1.validate that delet user 
+button not exist</t>
+  </si>
+  <si>
+    <t>delet user 
+button not exist</t>
   </si>
   <si>
     <t>TC_LearningHub_Follow_001</t>
@@ -2086,9 +1944,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -2172,19 +2030,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2195,10 +2044,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2218,8 +2068,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2248,21 +2099,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -2279,8 +2115,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2294,13 +2147,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2308,9 +2160,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2381,19 +2239,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2411,7 +2275,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2423,7 +2311,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2435,7 +2377,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2447,85 +2395,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2537,25 +2413,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2831,41 +2689,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2895,6 +2725,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2912,26 +2757,39 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2949,135 +2807,135 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3173,6 +3031,9 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -3206,11 +3067,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3595,7 +3459,7 @@
   <dimension ref="A1:L135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3641,7 +3505,7 @@
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -3653,10 +3517,10 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="48"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="11"/>
       <c r="K2" s="14"/>
       <c r="L2" s="11"/>
@@ -3665,7 +3529,7 @@
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -3677,10 +3541,10 @@
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="48"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="11"/>
       <c r="K3" s="14"/>
       <c r="L3" s="11"/>
@@ -3689,7 +3553,7 @@
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="52" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -3701,10 +3565,10 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="48"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="11"/>
       <c r="K4" s="14"/>
       <c r="L4" s="11"/>
@@ -3713,7 +3577,7 @@
       <c r="A5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -3725,10 +3589,10 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="48"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="11"/>
       <c r="K5" s="14"/>
       <c r="L5" s="11"/>
@@ -3737,7 +3601,7 @@
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="53" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -3749,10 +3613,10 @@
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="11"/>
       <c r="K6" s="14"/>
       <c r="L6" s="11"/>
@@ -3761,7 +3625,7 @@
       <c r="A7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -3773,10 +3637,10 @@
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="48"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="11"/>
       <c r="K7" s="14"/>
       <c r="L7" s="11"/>
@@ -3785,7 +3649,7 @@
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="53" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -3797,10 +3661,10 @@
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="48"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="11"/>
       <c r="K8" s="14"/>
       <c r="L8" s="11"/>
@@ -3809,7 +3673,7 @@
       <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -3821,335 +3685,335 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="47" t="s">
+      <c r="H9" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="48"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
       <c r="L9" s="11"/>
     </row>
     <row r="10" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="52"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="54"/>
     </row>
     <row r="11" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A11" s="56"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="56"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="58"/>
     </row>
     <row r="12" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="56"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="60"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="62"/>
     </row>
     <row r="14" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
     </row>
     <row r="15" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
     </row>
     <row r="16" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A16" s="65"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
     </row>
     <row r="20" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A20" s="65"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
     </row>
     <row r="22" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A22" s="65"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A23" s="65"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
     </row>
     <row r="24" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A24" s="65"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
     </row>
     <row r="25" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A25" s="65"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
     </row>
     <row r="26" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A26" s="65"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
     </row>
     <row r="27" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A27" s="65"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
     </row>
     <row r="28" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A28" s="65"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
     </row>
     <row r="29" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A29" s="65"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
     </row>
     <row r="30" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A30" s="65"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
     </row>
     <row r="31" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A31" s="65"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
     </row>
     <row r="32" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A32" s="65"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
     </row>
     <row r="33" ht="14.4" customHeight="1" spans="1:12">
       <c r="A33" s="2"/>
@@ -4454,456 +4318,456 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A13" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A15" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>341</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A17" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A18" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A19" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>354</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A20" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A22" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A23" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>363</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A24" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A25" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -4966,22 +4830,22 @@
       <c r="A2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="47" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="47" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="48"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="11"/>
       <c r="K2" s="14"/>
       <c r="L2" s="11"/>
@@ -4990,22 +4854,22 @@
       <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="47" t="s">
+      <c r="D3" s="50"/>
+      <c r="E3" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="47" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="48"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="11"/>
       <c r="K3" s="14"/>
       <c r="L3" s="11"/>
@@ -5014,22 +4878,22 @@
       <c r="A4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="47" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="47" t="s">
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="48"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="11"/>
       <c r="K4" s="14"/>
       <c r="L4" s="11"/>
@@ -5038,22 +4902,22 @@
       <c r="A5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="47" t="s">
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="48"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="11"/>
       <c r="K5" s="14"/>
       <c r="L5" s="11"/>
@@ -5062,22 +4926,22 @@
       <c r="A6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="47" t="s">
+      <c r="D6" s="50"/>
+      <c r="E6" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="47" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="11"/>
       <c r="K6" s="14"/>
       <c r="L6" s="11"/>
@@ -5086,22 +4950,22 @@
       <c r="A7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="47" t="s">
+      <c r="D7" s="50"/>
+      <c r="E7" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="47" t="s">
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="48"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="11"/>
       <c r="K7" s="14"/>
       <c r="L7" s="11"/>
@@ -5110,22 +4974,22 @@
       <c r="A8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="47" t="s">
+      <c r="D8" s="50"/>
+      <c r="E8" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="47" t="s">
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="48"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="11"/>
       <c r="K8" s="14"/>
       <c r="L8" s="11"/>
@@ -5134,347 +4998,347 @@
       <c r="A9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="47" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="47" t="s">
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="48"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
       <c r="L9" s="11"/>
     </row>
     <row r="10" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="52"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="54"/>
     </row>
     <row r="11" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A11" s="56"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="56"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="58"/>
     </row>
     <row r="12" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="56"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="60"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="62"/>
     </row>
     <row r="14" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
     </row>
     <row r="15" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
     </row>
     <row r="16" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A16" s="65"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
     </row>
     <row r="20" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A20" s="65"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
     </row>
     <row r="22" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A22" s="65"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A23" s="65"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
     </row>
     <row r="24" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A24" s="65"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
     </row>
     <row r="25" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A25" s="65"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
     </row>
     <row r="26" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A26" s="65"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
     </row>
     <row r="27" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A27" s="65"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
     </row>
     <row r="28" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A28" s="65"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
     </row>
     <row r="29" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A29" s="65"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
     </row>
     <row r="30" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A30" s="65"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
     </row>
     <row r="31" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A31" s="65"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
     </row>
     <row r="32" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A32" s="65"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
     </row>
     <row r="33" ht="14.4" customHeight="1" spans="1:12">
       <c r="A33" s="2"/>
@@ -5790,7 +5654,7 @@
       <c r="A2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="48" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -5802,10 +5666,10 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="48"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="11"/>
       <c r="K2" s="14"/>
       <c r="L2" s="11"/>
@@ -5814,7 +5678,7 @@
       <c r="A3" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="48" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -5826,10 +5690,10 @@
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="48"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="11"/>
       <c r="K3" s="14"/>
       <c r="L3" s="11"/>
@@ -5838,7 +5702,7 @@
       <c r="A4" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="48" t="s">
         <v>83</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -5850,10 +5714,10 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="48"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="11"/>
       <c r="K4" s="14"/>
       <c r="L4" s="11"/>
@@ -5862,7 +5726,7 @@
       <c r="A5" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="48" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -5874,10 +5738,10 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="48"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="11"/>
       <c r="K5" s="14"/>
       <c r="L5" s="11"/>
@@ -5886,7 +5750,7 @@
       <c r="A6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="48" t="s">
         <v>90</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -5898,10 +5762,10 @@
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="11"/>
       <c r="K6" s="14"/>
       <c r="L6" s="11"/>
@@ -5910,7 +5774,7 @@
       <c r="A7" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="48" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -5922,10 +5786,10 @@
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="48"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="11"/>
       <c r="K7" s="14"/>
       <c r="L7" s="11"/>
@@ -5934,7 +5798,7 @@
       <c r="A8" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="48" t="s">
         <v>97</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -5946,10 +5810,10 @@
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I8" s="48"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="11"/>
       <c r="K8" s="14"/>
       <c r="L8" s="11"/>
@@ -5958,7 +5822,7 @@
       <c r="A9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="48" t="s">
         <v>100</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -5970,10 +5834,10 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="47" t="s">
+      <c r="H9" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="I9" s="48"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
       <c r="L9" s="11"/>
@@ -5982,7 +5846,7 @@
       <c r="A10" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="48" t="s">
         <v>104</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -5994,10 +5858,10 @@
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="48"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="11"/>
       <c r="K10" s="14"/>
       <c r="L10" s="11"/>
@@ -6006,7 +5870,7 @@
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="48" t="s">
         <v>109</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -6018,10 +5882,10 @@
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="48"/>
+      <c r="I11" s="50"/>
       <c r="J11" s="11"/>
       <c r="K11" s="14"/>
       <c r="L11" s="11"/>
@@ -6030,7 +5894,7 @@
       <c r="A12" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="48" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -6042,10 +5906,10 @@
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="47" t="s">
+      <c r="H12" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="I12" s="48"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="11"/>
       <c r="K12" s="14"/>
       <c r="L12" s="11"/>
@@ -6054,7 +5918,7 @@
       <c r="A13" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="48" t="s">
         <v>118</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -6066,16 +5930,16 @@
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="48"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" ht="162.6" customHeight="1" spans="1:9">
       <c r="A14" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="48" t="s">
         <v>122</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -6087,16 +5951,16 @@
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="47" t="s">
+      <c r="H14" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="I14" s="48"/>
+      <c r="I14" s="50"/>
     </row>
     <row r="15" ht="193.8" customHeight="1" spans="1:9">
       <c r="A15" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="48" t="s">
         <v>125</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -6108,16 +5972,16 @@
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="I15" s="48"/>
+      <c r="I15" s="50"/>
     </row>
     <row r="16" ht="165" customHeight="1" spans="1:9">
       <c r="A16" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="48" t="s">
         <v>128</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -6129,16 +5993,16 @@
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="I16" s="48"/>
+      <c r="I16" s="50"/>
     </row>
     <row r="17" ht="165" customHeight="1" spans="1:9">
       <c r="A17" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="48" t="s">
         <v>132</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -6150,16 +6014,16 @@
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="47" t="s">
+      <c r="H17" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="I17" s="48"/>
+      <c r="I17" s="50"/>
     </row>
     <row r="18" ht="165" customHeight="1" spans="1:9">
       <c r="A18" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="48" t="s">
         <v>136</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -6171,32 +6035,32 @@
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="I18" s="48"/>
+      <c r="I18" s="50"/>
     </row>
     <row r="19" ht="165" customHeight="1" spans="1:9">
       <c r="A19" s="11"/>
-      <c r="B19" s="46"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="48"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
     </row>
     <row r="20" ht="165" customHeight="1" spans="1:9">
       <c r="A20" s="11"/>
-      <c r="B20" s="46"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="13"/>
       <c r="D20" s="14"/>
       <c r="E20" s="13"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="48"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="72">
@@ -6331,7 +6195,7 @@
       <c r="A2" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="48" t="s">
         <v>140</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -6343,10 +6207,10 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="48"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="11"/>
       <c r="K2" s="14"/>
       <c r="L2" s="11"/>
@@ -6355,7 +6219,7 @@
       <c r="A3" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="48" t="s">
         <v>144</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -6367,10 +6231,10 @@
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="48"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="11"/>
       <c r="K3" s="14"/>
       <c r="L3" s="11"/>
@@ -6379,7 +6243,7 @@
       <c r="A4" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="48" t="s">
         <v>148</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -6391,10 +6255,10 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="48"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="11"/>
       <c r="K4" s="14"/>
       <c r="L4" s="11"/>
@@ -6403,7 +6267,7 @@
       <c r="A5" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="48" t="s">
         <v>152</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -6415,108 +6279,108 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="I5" s="48"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="11"/>
       <c r="K5" s="14"/>
       <c r="L5" s="11"/>
     </row>
     <row r="6" ht="136.8" customHeight="1" spans="1:12">
       <c r="A6" s="11"/>
-      <c r="B6" s="46"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
       <c r="E6" s="13"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="11"/>
       <c r="K6" s="14"/>
       <c r="L6" s="11"/>
     </row>
     <row r="7" ht="136.8" customHeight="1" spans="1:12">
       <c r="A7" s="11"/>
-      <c r="B7" s="46"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14"/>
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="11"/>
       <c r="K7" s="14"/>
       <c r="L7" s="11"/>
     </row>
     <row r="8" ht="136.8" customHeight="1" spans="1:12">
       <c r="A8" s="11"/>
-      <c r="B8" s="46"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="11"/>
       <c r="K8" s="14"/>
       <c r="L8" s="11"/>
     </row>
     <row r="9" ht="136.8" customHeight="1" spans="1:12">
       <c r="A9" s="11"/>
-      <c r="B9" s="46"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
       <c r="L9" s="11"/>
     </row>
     <row r="10" ht="136.8" customHeight="1" spans="1:12">
       <c r="A10" s="11"/>
-      <c r="B10" s="46"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="13"/>
       <c r="D10" s="14"/>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="11"/>
       <c r="K10" s="14"/>
       <c r="L10" s="11"/>
     </row>
     <row r="11" ht="136.8" customHeight="1" spans="1:12">
       <c r="A11" s="11"/>
-      <c r="B11" s="46"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
       <c r="J11" s="11"/>
       <c r="K11" s="14"/>
       <c r="L11" s="11"/>
     </row>
     <row r="12" ht="136.8" customHeight="1" spans="1:12">
       <c r="A12" s="11"/>
-      <c r="B12" s="46"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="13"/>
       <c r="D12" s="14"/>
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="11"/>
       <c r="K12" s="14"/>
       <c r="L12" s="11"/>
@@ -6580,13 +6444,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="40.1047619047619" customWidth="1"/>
     <col min="2" max="2" width="26.6666666666667" customWidth="1"/>
@@ -6597,19 +6461,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="47.25" spans="1:7">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="18" t="s">
@@ -6619,100 +6483,110 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="190.05" customHeight="1" spans="1:7">
-      <c r="A2" s="37" t="s">
+    <row r="2" ht="238" customHeight="1" spans="1:7">
+      <c r="A2" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-    </row>
-    <row r="3" ht="165.75" spans="1:7">
-      <c r="A3" s="37" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" ht="180.75" spans="1:7">
+      <c r="A3" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" ht="228" customHeight="1" spans="1:7">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-    </row>
-    <row r="5" ht="165.75" spans="1:7">
-      <c r="A5" s="37" t="s">
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+    </row>
+    <row r="5" ht="235.95" customHeight="1" spans="1:7">
+      <c r="A5" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="E5" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-    </row>
-    <row r="6" ht="235.95" customHeight="1" spans="1:7">
-      <c r="A6" s="37" t="s">
+      <c r="E5" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+    </row>
+    <row r="6" s="33" customFormat="1" ht="240" customHeight="1" spans="1:5">
+      <c r="A6" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="C6" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="E6" s="46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:1">
+      <c r="A7" s="38"/>
+    </row>
+    <row r="8" ht="15.75" spans="1:1">
+      <c r="A8" s="38"/>
+    </row>
+    <row r="9" ht="15.75" spans="1:1">
+      <c r="A9" s="38"/>
+    </row>
+    <row r="10" ht="15.75" spans="1:1">
+      <c r="A10" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6765,76 +6639,76 @@
     </row>
     <row r="2" ht="199" customHeight="1" spans="1:7">
       <c r="A2" s="20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" ht="195" customHeight="1" spans="1:7">
       <c r="A3" s="20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
     <row r="4" ht="249" customHeight="1" spans="1:7">
       <c r="A4" s="20" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
     </row>
     <row r="5" ht="180.75" spans="1:7">
       <c r="A5" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
@@ -6905,22 +6779,22 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A2" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="11"/>
@@ -6929,22 +6803,22 @@
     </row>
     <row r="3" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A3" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="11"/>
@@ -6953,22 +6827,22 @@
     </row>
     <row r="4" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="11"/>
@@ -6977,22 +6851,22 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="11"/>
@@ -7001,22 +6875,22 @@
     </row>
     <row r="6" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="11"/>
@@ -7025,22 +6899,22 @@
     </row>
     <row r="7" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="11"/>
@@ -7133,22 +7007,22 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A2" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="11"/>
@@ -7157,22 +7031,22 @@
     </row>
     <row r="3" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A3" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="11"/>
@@ -7181,22 +7055,22 @@
     </row>
     <row r="4" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="11"/>
@@ -7205,22 +7079,22 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="11"/>
@@ -7229,22 +7103,22 @@
     </row>
     <row r="6" s="2" customFormat="1" ht="157.8" customHeight="1" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="11"/>
@@ -7329,260 +7203,260 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="96" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="91.2" customHeight="1" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="87" customHeight="1" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="96.6" customHeight="1" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="102" customHeight="1" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="100.2" customHeight="1" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="99.6" customHeight="1" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="95.4" customHeight="1" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="94.2" customHeight="1" spans="1:7">
       <c r="A10" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>282</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="95.4" customHeight="1" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="94.2" customHeight="1" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="94.8" customHeight="1" spans="1:7">
       <c r="A13" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="102.6" customHeight="1" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="94.8" customHeight="1" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>

</xml_diff>

<commit_message>
Change title in TC of follow feature
</commit_message>
<xml_diff>
--- a/Testing/Test Report/TestCases.xlsx
+++ b/Testing/Test Report/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -971,7 +971,7 @@
     <t>TC_LearningHub_Follow_001</t>
   </si>
   <si>
-    <t>Follow a Category Page successfully</t>
+    <t>User can select a Category Page  and follow it successfully</t>
   </si>
   <si>
     <r>
@@ -1084,7 +1084,7 @@
     <t>TC_LearningHub_Follow_002</t>
   </si>
   <si>
-    <t>Unfollow a Category Page successfully</t>
+    <t>User can select a cateogry page "already follow it "and  unfollow it successfully</t>
   </si>
   <si>
     <r>
@@ -1169,34 +1169,7 @@
     <t>TC_LearningHub_Follow_003</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>prevent following the same category</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>page twice</t>
-    </r>
+    <t>User can' follow the same category page twice</t>
   </si>
   <si>
     <r>
@@ -1264,34 +1237,8 @@
     <t>TC_LearningHub_Follow_004</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF050E17"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Prevent unfollowing a category page that </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF050E17"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF050E17"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>has not been followed</t>
-    </r>
+    <t>User can't unfollow a category page that 
+has not been followed</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -2002,10 +1949,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -2103,9 +2050,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2119,24 +2066,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2159,14 +2106,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2196,18 +2136,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2218,7 +2158,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2226,8 +2172,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2298,13 +2245,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2316,121 +2395,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2448,37 +2419,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2748,17 +2695,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2813,24 +2749,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2845,152 +2763,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6498,7 +6445,7 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -6641,8 +6588,8 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -6755,7 +6702,7 @@
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
     </row>
-    <row r="6" ht="15.75" spans="1:7">
+    <row r="6" spans="1:7">
       <c r="A6" s="20"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>

</xml_diff>

<commit_message>
add del user & follow test case to RTM
</commit_message>
<xml_diff>
--- a/Testing/Test Report/TestCases.xlsx
+++ b/Testing/Test Report/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" activeTab="4"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -863,6 +863,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>admin can't delete user by entering email not attached to the entered username</t>
     </r>
     <r>
@@ -1878,12 +1885,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1966,13 +1973,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2028,9 +2028,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2050,9 +2065,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2066,32 +2081,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2106,8 +2098,30 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2118,28 +2132,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2158,8 +2150,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2172,11 +2165,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2243,7 +2235,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2255,7 +2283,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2267,31 +2379,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2303,121 +2409,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2713,6 +2705,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2738,6 +2741,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2754,11 +2772,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2768,30 +2784,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2813,7 +2805,7 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2834,132 +2826,132 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="29" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="29" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="30" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="30" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3106,43 +3098,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="32" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="32" applyBorder="1" applyAlignment="1">
@@ -3163,34 +3152,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="32" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="32" applyBorder="1" applyAlignment="1">
@@ -3205,10 +3194,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3550,566 +3539,566 @@
   </cols>
   <sheetData>
     <row r="1" ht="31.5" spans="1:12">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="71" t="s">
+      <c r="D1" s="71"/>
+      <c r="E1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="71" t="s">
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="83" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="72"/>
-      <c r="L1" s="83" t="s">
+      <c r="K1" s="71"/>
+      <c r="L1" s="82" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="157.95" customHeight="1" spans="1:12">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="74" t="s">
+      <c r="D2" s="74"/>
+      <c r="E2" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="74" t="s">
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="51"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="50"/>
     </row>
     <row r="3" ht="183.6" customHeight="1" spans="1:12">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="74" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="74" t="s">
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="75"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="51"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="50"/>
     </row>
     <row r="4" ht="143.4" customHeight="1" spans="1:12">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="74" t="s">
+      <c r="D4" s="74"/>
+      <c r="E4" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="74" t="s">
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="75"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="51"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="50"/>
     </row>
     <row r="5" ht="158.4" customHeight="1" spans="1:12">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="74" t="s">
+      <c r="D5" s="74"/>
+      <c r="E5" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="74" t="s">
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="75"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="51"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="50"/>
     </row>
     <row r="6" ht="144" customHeight="1" spans="1:12">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="74" t="s">
+      <c r="D6" s="74"/>
+      <c r="E6" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="74" t="s">
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="51"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" ht="154.95" customHeight="1" spans="1:12">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="74" t="s">
+      <c r="D7" s="74"/>
+      <c r="E7" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="74" t="s">
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="51"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="50"/>
     </row>
     <row r="8" ht="145.95" customHeight="1" spans="1:12">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="78"/>
-      <c r="E8" s="74" t="s">
+      <c r="D8" s="77"/>
+      <c r="E8" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="74" t="s">
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="51"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="50"/>
     </row>
     <row r="9" ht="156.6" customHeight="1" spans="1:12">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="74" t="s">
+      <c r="D9" s="74"/>
+      <c r="E9" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="74" t="s">
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="75"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="51"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" ht="184.8" customHeight="1" spans="1:12">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="75"/>
-      <c r="E10" s="74" t="s">
+      <c r="D10" s="74"/>
+      <c r="E10" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="74" t="s">
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="75"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="51"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="50"/>
     </row>
     <row r="11" ht="235.2" customHeight="1" spans="1:12">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="75"/>
-      <c r="E11" s="74" t="s">
+      <c r="D11" s="74"/>
+      <c r="E11" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="74" t="s">
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="75"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="51"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="50"/>
     </row>
     <row r="12" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="79"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="78"/>
     </row>
     <row r="13" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="63"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="62"/>
     </row>
     <row r="14" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A14" s="68"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
     </row>
     <row r="15" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A15" s="68"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
     </row>
     <row r="16" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A16" s="68"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A17" s="68"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A19" s="68"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
     </row>
     <row r="20" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A21" s="68"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
     </row>
     <row r="22" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A22" s="68"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A23" s="68"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
     </row>
     <row r="24" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A24" s="68"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
     </row>
     <row r="25" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A25" s="68"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="68"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
     </row>
     <row r="26" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A26" s="68"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
     </row>
     <row r="27" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A27" s="68"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
     </row>
     <row r="28" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A28" s="68"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
     </row>
     <row r="29" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A29" s="68"/>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
     </row>
     <row r="30" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A30" s="68"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
     </row>
     <row r="31" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
     </row>
     <row r="32" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A32" s="68"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
     </row>
     <row r="33" ht="14.4" customHeight="1" spans="1:12">
       <c r="A33" s="2"/>
@@ -4894,7 +4883,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" spans="1:12">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -4922,562 +4911,562 @@
       </c>
     </row>
     <row r="2" ht="157.95" customHeight="1" spans="1:12">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="53" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="69"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="68"/>
     </row>
     <row r="3" ht="148.2" customHeight="1" spans="1:12">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="53" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="53" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="69"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="68"/>
     </row>
     <row r="4" ht="143.4" customHeight="1" spans="1:12">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="53" t="s">
+      <c r="D4" s="53"/>
+      <c r="E4" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="53" t="s">
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="54"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="69"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="68"/>
     </row>
     <row r="5" ht="143.4" customHeight="1" spans="1:12">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="53" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="53" t="s">
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="69"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="68"/>
     </row>
     <row r="6" ht="158.4" customHeight="1" spans="1:12">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="53" t="s">
+      <c r="D6" s="53"/>
+      <c r="E6" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="53" t="s">
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="69"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="68"/>
     </row>
     <row r="7" ht="144" customHeight="1" spans="1:12">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="53" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="53" t="s">
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="69"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="68"/>
     </row>
     <row r="8" ht="144" customHeight="1" spans="1:12">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="53" t="s">
+      <c r="D8" s="53"/>
+      <c r="E8" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="53" t="s">
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="69"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="68"/>
     </row>
     <row r="9" ht="154.95" customHeight="1" spans="1:12">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="53" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="53" t="s">
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="54"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="69"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="68"/>
     </row>
     <row r="10" ht="154.95" customHeight="1" spans="1:12">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="53" t="s">
+      <c r="D10" s="53"/>
+      <c r="E10" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="53" t="s">
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="69"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="68"/>
     </row>
     <row r="11" ht="157.95" customHeight="1" spans="1:12">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="53" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="53" t="s">
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="54"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="69"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="68"/>
     </row>
     <row r="12" ht="157.95" customHeight="1" spans="1:12">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="53" t="s">
+      <c r="D12" s="53"/>
+      <c r="E12" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="53" t="s">
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="54"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="69"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="68"/>
     </row>
     <row r="13" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A13" s="58"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="59"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="58"/>
     </row>
     <row r="14" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="63"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="62"/>
     </row>
     <row r="15" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A15" s="68"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
     </row>
     <row r="16" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A16" s="68"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A17" s="68"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A19" s="68"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
     </row>
     <row r="20" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A21" s="68"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
     </row>
     <row r="22" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A22" s="68"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A23" s="68"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
     </row>
     <row r="24" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A24" s="68"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
     </row>
     <row r="25" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A25" s="68"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="68"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
     </row>
     <row r="26" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A26" s="68"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
     </row>
     <row r="27" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A27" s="68"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
     </row>
     <row r="28" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A28" s="68"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
     </row>
     <row r="29" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A29" s="68"/>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
     </row>
     <row r="30" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A30" s="68"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
     </row>
     <row r="31" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
     </row>
     <row r="32" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A32" s="68"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
     </row>
     <row r="33" ht="14.4" customHeight="1" spans="1:12">
-      <c r="A33" s="68"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
     </row>
     <row r="34" ht="14.4" customHeight="1" spans="1:12">
       <c r="A34" s="2"/>
@@ -6589,7 +6578,7 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -6753,8 +6742,8 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -6883,7 +6872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" ht="15.75" spans="1:7">
       <c r="A6" s="20"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>

</xml_diff>